<commit_message>
provenance buttoned up with url
</commit_message>
<xml_diff>
--- a/python/xlsx/python XL test.xlsx
+++ b/python/xlsx/python XL test.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Created by</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>AMANZI: The Multi-Process HPC Simulator</t>
+  </si>
+  <si>
+    <t>Workbook created by</t>
   </si>
   <si>
     <t>python source</t>
@@ -90,10 +93,28 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yy/mm/dd hh:mm"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,13 +137,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,150 +444,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
-      </c>
-      <c r="B9">
-        <v>43430.87504807177</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="B12" s="3">
+        <v>43430.89295642584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B13">
-        <f> INFO( "system" )</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <f> INFO( "recalc" )</f>
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <f> INFO( "numfile" )</f>
+        <f> INFO( "system" )</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <f> INFO( "origin" )</f>
+        <f> INFO( "recalc" )</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <f> INFO( "release" )</f>
+        <f> INFO( "numfile" )</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
-        <f> INFO( "directory" )</f>
+        <f> INFO( "origin" )</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <f> INFO( "release" )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B19">
+      <c r="B20">
+        <f> INFO( "directory" )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
         <f> INFO( "osversion" )</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;12&amp;A</oddHeader>

</xml_diff>

<commit_message>
tag delta, move to echo
</commit_message>
<xml_diff>
--- a/python/xlsx/python XL test.xlsx
+++ b/python/xlsx/python XL test.xlsx
@@ -1,26 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dantopa/Documents/repos/GitHub/topa-development/python/xlsx/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85096F1A-EF8E-354D-A321-2027D32F8D61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="provenance" sheetId="1" r:id="rId1"/>
+    <sheet name="requirements - PASS" sheetId="2" r:id="rId2"/>
+    <sheet name="requirements - FAIL" sheetId="3" r:id="rId3"/>
+    <sheet name="requirements - NULL" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>AMANZI: The Multi-Process HPC Simulator</t>
   </si>
@@ -94,15 +91,24 @@
   <si>
     <t>operating systems</t>
   </si>
+  <si>
+    <t>Summary or requirements PASSED</t>
+  </si>
+  <si>
+    <t>Summary or requirements FAIL</t>
+  </si>
+  <si>
+    <t>Summary or requirements NULL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yy/mm/dd\ hh:mm"/>
+    <numFmt numFmtId="164" formatCode="yy/mm/dd hh:mm"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,14 +168,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -216,7 +214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,27 +246,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -300,24 +280,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -493,28 +455,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -522,7 +484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -530,7 +492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -538,12 +500,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -551,7 +513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -559,7 +521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -567,85 +529,85 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3">
-        <v>43430.892956425843</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>43431.21433859861</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="str">
-        <f ca="1">INFO( "system" )</f>
-        <v>mac</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f> INFO( "system" )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="str">
-        <f ca="1">INFO( "recalc" )</f>
-        <v>Automatic</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f> INFO( "recalc" )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17">
-        <f ca="1">INFO( "numfile" )</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <f> INFO( "numfile" )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="str">
-        <f ca="1">INFO( "origin" )</f>
-        <v>$A:$A$1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <f> INFO( "origin" )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" t="str">
-        <f ca="1">INFO( "release" )</f>
-        <v>16.16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f> INFO( "release" )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="str">
-        <f ca="1">INFO( "directory" )</f>
-        <v>/Users/dantopa/Library/Containers/com.microsoft.Excel/Data/Documents/</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f> INFO( "directory" )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="str">
-        <f ca="1">INFO( "osversion" )</f>
-        <v>Macintosh (Intel) Version 10.13.3 (Build 17D47)</v>
+      <c r="B21">
+        <f> INFO( "osversion" )</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -655,4 +617,76 @@
 &amp;8&amp;F</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;L&amp;8&amp;T
+&amp;8&amp;D&amp;C &amp;P / &amp;N&amp;R&amp;8&amp;Z
+&amp;8&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;L&amp;8&amp;T
+&amp;8&amp;D&amp;C &amp;P / &amp;N&amp;R&amp;8&amp;Z
+&amp;8&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;L&amp;8&amp;T
+&amp;8&amp;D&amp;C &amp;P / &amp;N&amp;R&amp;8&amp;Z
+&amp;8&amp;F</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
all is well: amanzi/aqua/xl/wtf.py
</commit_message>
<xml_diff>
--- a/python/xlsx/python XL test.xlsx
+++ b/python/xlsx/python XL test.xlsx
@@ -34,14 +34,14 @@
     <t>directory</t>
   </si>
   <si>
-    <t>/Users/dantopa/Documents/repos/GitHub/topa-development/python/xlsx</t>
+    <t>/Volumes/Tlaltecuhtli/repos/GitHub/topa-development/python/xlsx</t>
   </si>
   <si>
     <t>python version</t>
   </si>
   <si>
-    <t>3.6.7 (default, Oct 21 2018, 09:26:25) 
-[GCC 4.2.1 Compatible Apple LLVM 9.1.0 (clang-902.0.39.2)]</t>
+    <t>3.7.0 (default, Jun 28 2018, 07:39:16) 
+[Clang 4.0.1 (tags/RELEASE_401/final)]</t>
   </si>
   <si>
     <t>Environment variables</t>
@@ -50,19 +50,19 @@
     <t>$USER</t>
   </si>
   <si>
-    <t>dantopa</t>
+    <t>l127914</t>
   </si>
   <si>
     <t>$HOSTNAME</t>
   </si>
   <si>
-    <t>MacBookPro11,3</t>
+    <t>Cauchy.Schwarz</t>
   </si>
   <si>
     <t>$HOME</t>
   </si>
   <si>
-    <t>/Users/dantopa</t>
+    <t>/Users/l127914</t>
   </si>
   <si>
     <t>timestamp</t>
@@ -534,7 +534,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="3">
-        <v>43431.21572409587</v>
+        <v>43438.43873602271</v>
       </c>
     </row>
     <row r="14" spans="1:2">

</xml_diff>